<commit_message>
added mul tickers and general fixes
</commit_message>
<xml_diff>
--- a/model/qml_experiment_log.xlsx
+++ b/model/qml_experiment_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y11"/>
+  <dimension ref="A1:Z20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -559,6 +559,11 @@
           <t>Notes</t>
         </is>
       </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>Tickers</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -640,6 +645,7 @@
           <t>Test on more dynamic data, add dropout and layernorm.</t>
         </is>
       </c>
+      <c r="Z2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -717,6 +723,7 @@
           <t>Test on more dynamic data, add dropout and layernorm.</t>
         </is>
       </c>
+      <c r="Z3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -790,6 +797,7 @@
       </c>
       <c r="X4" t="inlineStr"/>
       <c r="Y4" t="inlineStr"/>
+      <c r="Z4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -863,6 +871,7 @@
       </c>
       <c r="X5" t="inlineStr"/>
       <c r="Y5" t="inlineStr"/>
+      <c r="Z5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -946,6 +955,7 @@
           <t>Classical Run with LSTM, no dropout, no layernorm, no quantum layer</t>
         </is>
       </c>
+      <c r="Z6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -1023,6 +1033,7 @@
           <t>run with Quantum layer</t>
         </is>
       </c>
+      <c r="Z7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -1100,6 +1111,7 @@
           <t>run with Quantum layer</t>
         </is>
       </c>
+      <c r="Z8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -1177,6 +1189,7 @@
           <t>run with Quantum layer</t>
         </is>
       </c>
+      <c r="Z9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -1256,6 +1269,7 @@
           <t>run with Quantum layer</t>
         </is>
       </c>
+      <c r="Z10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -1333,6 +1347,739 @@
       <c r="Y11" t="inlineStr">
         <is>
           <t>run with Quantum layer</t>
+        </is>
+      </c>
+      <c r="Z11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Auto-log: Q=2, D=2, Skip=concat</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>2</v>
+      </c>
+      <c r="D12" t="n">
+        <v>1</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" t="n">
+        <v>16</v>
+      </c>
+      <c r="G12" t="n">
+        <v>20</v>
+      </c>
+      <c r="H12" t="b">
+        <v>1</v>
+      </c>
+      <c r="I12" t="n">
+        <v>2</v>
+      </c>
+      <c r="J12" t="n">
+        <v>2</v>
+      </c>
+      <c r="K12" t="n">
+        <v>3</v>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>concat</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr"/>
+      <c r="N12" t="b">
+        <v>0</v>
+      </c>
+      <c r="O12" t="n">
+        <v>0</v>
+      </c>
+      <c r="P12" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q12" t="inlineStr"/>
+      <c r="R12" t="n">
+        <v>15</v>
+      </c>
+      <c r="S12" t="n">
+        <v>2</v>
+      </c>
+      <c r="T12" t="n">
+        <v>0.0002755922186123725</v>
+      </c>
+      <c r="U12" t="n">
+        <v>0.008164557970303576</v>
+      </c>
+      <c r="V12" t="n">
+        <v>14.92195510864258</v>
+      </c>
+      <c r="W12" t="n">
+        <v>19.71026420593262</v>
+      </c>
+      <c r="X12" t="n">
+        <v>7.186328411102295</v>
+      </c>
+      <c r="Y12" t="inlineStr">
+        <is>
+          <t>run with Quantum layer</t>
+        </is>
+      </c>
+      <c r="Z12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Auto-log: Q=2, D=2, Skip=concat</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>2</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" t="n">
+        <v>16</v>
+      </c>
+      <c r="G13" t="n">
+        <v>20</v>
+      </c>
+      <c r="H13" t="b">
+        <v>1</v>
+      </c>
+      <c r="I13" t="n">
+        <v>2</v>
+      </c>
+      <c r="J13" t="n">
+        <v>2</v>
+      </c>
+      <c r="K13" t="n">
+        <v>3</v>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>concat</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr"/>
+      <c r="N13" t="b">
+        <v>0</v>
+      </c>
+      <c r="O13" t="n">
+        <v>0</v>
+      </c>
+      <c r="P13" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q13" t="inlineStr"/>
+      <c r="R13" t="n">
+        <v>15</v>
+      </c>
+      <c r="S13" t="n">
+        <v>2</v>
+      </c>
+      <c r="T13" t="n">
+        <v>0.0002311510873527917</v>
+      </c>
+      <c r="U13" t="n">
+        <v>0.006108876623329706</v>
+      </c>
+      <c r="V13" t="n">
+        <v>12.91889095306396</v>
+      </c>
+      <c r="W13" t="n">
+        <v>17.25859451293945</v>
+      </c>
+      <c r="X13" t="n">
+        <v>6.20987606048584</v>
+      </c>
+      <c r="Y13" t="inlineStr">
+        <is>
+          <t>run with Quantum layer</t>
+        </is>
+      </c>
+      <c r="Z13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Auto-log: Q=2, D=2, Skip=concat</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>4</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" t="n">
+        <v>16</v>
+      </c>
+      <c r="G14" t="n">
+        <v>20</v>
+      </c>
+      <c r="H14" t="b">
+        <v>1</v>
+      </c>
+      <c r="I14" t="n">
+        <v>2</v>
+      </c>
+      <c r="J14" t="n">
+        <v>2</v>
+      </c>
+      <c r="K14" t="n">
+        <v>3</v>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>concat</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr"/>
+      <c r="N14" t="b">
+        <v>0</v>
+      </c>
+      <c r="O14" t="n">
+        <v>0</v>
+      </c>
+      <c r="P14" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q14" t="inlineStr"/>
+      <c r="R14" t="n">
+        <v>15</v>
+      </c>
+      <c r="S14" t="n">
+        <v>2</v>
+      </c>
+      <c r="T14" t="n">
+        <v>0.0006707275329279669</v>
+      </c>
+      <c r="U14" t="n">
+        <v>0.01115978131565498</v>
+      </c>
+      <c r="V14" t="n">
+        <v>15.28087520599365</v>
+      </c>
+      <c r="W14" t="n">
+        <v>21.42845153808594</v>
+      </c>
+      <c r="X14" t="n">
+        <v>7.279820442199707</v>
+      </c>
+      <c r="Y14" t="inlineStr">
+        <is>
+          <t>run with Quantum layer</t>
+        </is>
+      </c>
+      <c r="Z14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Auto-log: Q=2, D=2, Skip=concat</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>4</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" t="n">
+        <v>16</v>
+      </c>
+      <c r="G15" t="n">
+        <v>20</v>
+      </c>
+      <c r="H15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I15" t="n">
+        <v>2</v>
+      </c>
+      <c r="J15" t="n">
+        <v>2</v>
+      </c>
+      <c r="K15" t="n">
+        <v>3</v>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>concat</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr"/>
+      <c r="N15" t="b">
+        <v>0</v>
+      </c>
+      <c r="O15" t="n">
+        <v>0</v>
+      </c>
+      <c r="P15" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q15" t="inlineStr"/>
+      <c r="R15" t="n">
+        <v>15</v>
+      </c>
+      <c r="S15" t="n">
+        <v>2</v>
+      </c>
+      <c r="T15" t="n">
+        <v>1.132239412982017e-05</v>
+      </c>
+      <c r="U15" t="n">
+        <v>5.341193536878563e-05</v>
+      </c>
+      <c r="V15" t="n">
+        <v>0.1708307266235352</v>
+      </c>
+      <c r="W15" t="n">
+        <v>0.1843285113573074</v>
+      </c>
+      <c r="X15" t="n">
+        <v>0.60400390625</v>
+      </c>
+      <c r="Y15" t="inlineStr">
+        <is>
+          <t>run with Quantum layer</t>
+        </is>
+      </c>
+      <c r="Z15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Auto-log: Q=2, D=2, Skip=concat</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>4</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" t="n">
+        <v>16</v>
+      </c>
+      <c r="G16" t="n">
+        <v>20</v>
+      </c>
+      <c r="H16" t="b">
+        <v>1</v>
+      </c>
+      <c r="I16" t="n">
+        <v>2</v>
+      </c>
+      <c r="J16" t="n">
+        <v>2</v>
+      </c>
+      <c r="K16" t="n">
+        <v>3</v>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>concat</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr"/>
+      <c r="N16" t="b">
+        <v>0</v>
+      </c>
+      <c r="O16" t="n">
+        <v>0</v>
+      </c>
+      <c r="P16" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q16" t="inlineStr"/>
+      <c r="R16" t="n">
+        <v>15</v>
+      </c>
+      <c r="S16" t="n">
+        <v>2</v>
+      </c>
+      <c r="T16" t="n">
+        <v>0.0006707280517152939</v>
+      </c>
+      <c r="U16" t="n">
+        <v>0.01115977805784496</v>
+      </c>
+      <c r="V16" t="n">
+        <v>15.28087711334229</v>
+      </c>
+      <c r="W16" t="n">
+        <v>21.42845344543457</v>
+      </c>
+      <c r="X16" t="n">
+        <v>7.279821395874023</v>
+      </c>
+      <c r="Y16" t="inlineStr">
+        <is>
+          <t>run with Quantum layer</t>
+        </is>
+      </c>
+      <c r="Z16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Auto-log: Q=2, D=2, Skip=concat</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>4</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" t="n">
+        <v>16</v>
+      </c>
+      <c r="G17" t="n">
+        <v>20</v>
+      </c>
+      <c r="H17" t="b">
+        <v>1</v>
+      </c>
+      <c r="I17" t="n">
+        <v>2</v>
+      </c>
+      <c r="J17" t="n">
+        <v>2</v>
+      </c>
+      <c r="K17" t="n">
+        <v>3</v>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>concat</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr"/>
+      <c r="N17" t="b">
+        <v>0</v>
+      </c>
+      <c r="O17" t="n">
+        <v>0</v>
+      </c>
+      <c r="P17" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q17" t="inlineStr"/>
+      <c r="R17" t="n">
+        <v>15</v>
+      </c>
+      <c r="S17" t="n">
+        <v>2</v>
+      </c>
+      <c r="T17" t="n">
+        <v>0.0002620218473702095</v>
+      </c>
+      <c r="U17" t="n">
+        <v>0.0008594085127387711</v>
+      </c>
+      <c r="V17" t="n">
+        <v>3.520127534866333</v>
+      </c>
+      <c r="W17" t="n">
+        <v>4.569629192352295</v>
+      </c>
+      <c r="X17" t="n">
+        <v>2.406062841415405</v>
+      </c>
+      <c r="Y17" t="inlineStr">
+        <is>
+          <t>run with Quantum layer</t>
+        </is>
+      </c>
+      <c r="Z17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Auto-log: Q=2, D=2, Skip=concat</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>4</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" t="n">
+        <v>16</v>
+      </c>
+      <c r="G18" t="n">
+        <v>20</v>
+      </c>
+      <c r="H18" t="b">
+        <v>1</v>
+      </c>
+      <c r="I18" t="n">
+        <v>2</v>
+      </c>
+      <c r="J18" t="n">
+        <v>2</v>
+      </c>
+      <c r="K18" t="n">
+        <v>3</v>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>concat</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr"/>
+      <c r="N18" t="b">
+        <v>0</v>
+      </c>
+      <c r="O18" t="n">
+        <v>0</v>
+      </c>
+      <c r="P18" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q18" t="inlineStr"/>
+      <c r="R18" t="n">
+        <v>15</v>
+      </c>
+      <c r="S18" t="n">
+        <v>2</v>
+      </c>
+      <c r="T18" t="n">
+        <v>0.0002620218473702095</v>
+      </c>
+      <c r="U18" t="n">
+        <v>0.0008594085127387711</v>
+      </c>
+      <c r="V18" t="n">
+        <v>3.520127534866333</v>
+      </c>
+      <c r="W18" t="n">
+        <v>4.569629192352295</v>
+      </c>
+      <c r="X18" t="n">
+        <v>2.406062841415405</v>
+      </c>
+      <c r="Y18" t="inlineStr">
+        <is>
+          <t>Multi-ticker experiment with LSTM+Quantum</t>
+        </is>
+      </c>
+      <c r="Z18" t="inlineStr">
+        <is>
+          <t>AAPL, MSFT, GOOGL</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Auto-log: Q=2, D=2, Skip=concat</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>4</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" t="n">
+        <v>16</v>
+      </c>
+      <c r="G19" t="n">
+        <v>20</v>
+      </c>
+      <c r="H19" t="b">
+        <v>1</v>
+      </c>
+      <c r="I19" t="n">
+        <v>2</v>
+      </c>
+      <c r="J19" t="n">
+        <v>2</v>
+      </c>
+      <c r="K19" t="n">
+        <v>3</v>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>concat</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr"/>
+      <c r="N19" t="b">
+        <v>0</v>
+      </c>
+      <c r="O19" t="n">
+        <v>0</v>
+      </c>
+      <c r="P19" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q19" t="inlineStr"/>
+      <c r="R19" t="n">
+        <v>15</v>
+      </c>
+      <c r="S19" t="n">
+        <v>2</v>
+      </c>
+      <c r="T19" t="n">
+        <v>0.0002620218473702095</v>
+      </c>
+      <c r="U19" t="n">
+        <v>0.0008594085127387711</v>
+      </c>
+      <c r="V19" t="n">
+        <v>3.520127534866333</v>
+      </c>
+      <c r="W19" t="n">
+        <v>4.569629192352295</v>
+      </c>
+      <c r="X19" t="n">
+        <v>2.406062841415405</v>
+      </c>
+      <c r="Y19" t="inlineStr">
+        <is>
+          <t>run with Quantum layer</t>
+        </is>
+      </c>
+      <c r="Z19" t="inlineStr">
+        <is>
+          <t>AAPL, MSFT, GOOGL</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Auto-log: Q=2, D=2, Skip=concat</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>4</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" t="n">
+        <v>16</v>
+      </c>
+      <c r="G20" t="n">
+        <v>20</v>
+      </c>
+      <c r="H20" t="b">
+        <v>1</v>
+      </c>
+      <c r="I20" t="n">
+        <v>2</v>
+      </c>
+      <c r="J20" t="n">
+        <v>2</v>
+      </c>
+      <c r="K20" t="n">
+        <v>3</v>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>concat</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr"/>
+      <c r="N20" t="b">
+        <v>0</v>
+      </c>
+      <c r="O20" t="n">
+        <v>0</v>
+      </c>
+      <c r="P20" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q20" t="inlineStr"/>
+      <c r="R20" t="n">
+        <v>15</v>
+      </c>
+      <c r="S20" t="n">
+        <v>2</v>
+      </c>
+      <c r="T20" t="n">
+        <v>0.0002620216811455395</v>
+      </c>
+      <c r="U20" t="n">
+        <v>0.0008594098481092047</v>
+      </c>
+      <c r="V20" t="n">
+        <v>3.520127534866333</v>
+      </c>
+      <c r="W20" t="n">
+        <v>4.569628238677979</v>
+      </c>
+      <c r="X20" t="n">
+        <v>2.406063079833984</v>
+      </c>
+      <c r="Y20" t="inlineStr">
+        <is>
+          <t>run with Quantum layer</t>
+        </is>
+      </c>
+      <c r="Z20" t="inlineStr">
+        <is>
+          <t>AAPL, MSFT, GOOGL</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
trying to optimize & save good notebook
</commit_message>
<xml_diff>
--- a/model/qml_experiment_log.xlsx
+++ b/model/qml_experiment_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Z20"/>
+  <dimension ref="A1:Z25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2083,6 +2083,426 @@
         </is>
       </c>
     </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Auto-log: Q=2, D=2, Skip=concat</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>4</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" t="n">
+        <v>16</v>
+      </c>
+      <c r="G21" t="n">
+        <v>20</v>
+      </c>
+      <c r="H21" t="b">
+        <v>1</v>
+      </c>
+      <c r="I21" t="n">
+        <v>2</v>
+      </c>
+      <c r="J21" t="n">
+        <v>2</v>
+      </c>
+      <c r="K21" t="n">
+        <v>3</v>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>concat</t>
+        </is>
+      </c>
+      <c r="M21" t="inlineStr"/>
+      <c r="N21" t="b">
+        <v>0</v>
+      </c>
+      <c r="O21" t="n">
+        <v>0</v>
+      </c>
+      <c r="P21" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q21" t="inlineStr"/>
+      <c r="R21" t="n">
+        <v>15</v>
+      </c>
+      <c r="S21" t="n">
+        <v>2</v>
+      </c>
+      <c r="T21" t="n">
+        <v>0.0002620218950122511</v>
+      </c>
+      <c r="U21" t="n">
+        <v>0.0008594071114202961</v>
+      </c>
+      <c r="V21" t="n">
+        <v>3.520127534866333</v>
+      </c>
+      <c r="W21" t="n">
+        <v>4.569628238677979</v>
+      </c>
+      <c r="X21" t="n">
+        <v>2.40606427192688</v>
+      </c>
+      <c r="Y21" t="inlineStr">
+        <is>
+          <t>run with Quantum layer</t>
+        </is>
+      </c>
+      <c r="Z21" t="inlineStr">
+        <is>
+          <t>AAPL, MSFT, GOOGL</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Auto-log: Q=2, D=2, Skip=concat</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>4</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0</v>
+      </c>
+      <c r="F22" t="n">
+        <v>16</v>
+      </c>
+      <c r="G22" t="n">
+        <v>20</v>
+      </c>
+      <c r="H22" t="b">
+        <v>1</v>
+      </c>
+      <c r="I22" t="n">
+        <v>2</v>
+      </c>
+      <c r="J22" t="n">
+        <v>2</v>
+      </c>
+      <c r="K22" t="n">
+        <v>3</v>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>concat</t>
+        </is>
+      </c>
+      <c r="M22" t="inlineStr"/>
+      <c r="N22" t="b">
+        <v>0</v>
+      </c>
+      <c r="O22" t="n">
+        <v>0</v>
+      </c>
+      <c r="P22" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q22" t="inlineStr"/>
+      <c r="R22" t="n">
+        <v>15</v>
+      </c>
+      <c r="S22" t="n">
+        <v>2</v>
+      </c>
+      <c r="T22" t="n">
+        <v>0.0002620217367988749</v>
+      </c>
+      <c r="U22" t="n">
+        <v>0.00085940357437605</v>
+      </c>
+      <c r="V22" t="n">
+        <v>3.520126819610596</v>
+      </c>
+      <c r="W22" t="n">
+        <v>4.569628238677979</v>
+      </c>
+      <c r="X22" t="n">
+        <v>2.40606427192688</v>
+      </c>
+      <c r="Y22" t="inlineStr">
+        <is>
+          <t>run with Quantum layer</t>
+        </is>
+      </c>
+      <c r="Z22" t="inlineStr">
+        <is>
+          <t>AAPL, MSFT, GOOGL</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Auto-log: Q=2, D=2, Skip=concat</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>4</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0</v>
+      </c>
+      <c r="F23" t="n">
+        <v>16</v>
+      </c>
+      <c r="G23" t="n">
+        <v>20</v>
+      </c>
+      <c r="H23" t="b">
+        <v>1</v>
+      </c>
+      <c r="I23" t="n">
+        <v>2</v>
+      </c>
+      <c r="J23" t="n">
+        <v>2</v>
+      </c>
+      <c r="K23" t="n">
+        <v>3</v>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>concat</t>
+        </is>
+      </c>
+      <c r="M23" t="inlineStr"/>
+      <c r="N23" t="b">
+        <v>0</v>
+      </c>
+      <c r="O23" t="n">
+        <v>0</v>
+      </c>
+      <c r="P23" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q23" t="inlineStr"/>
+      <c r="R23" t="n">
+        <v>15</v>
+      </c>
+      <c r="S23" t="n">
+        <v>2</v>
+      </c>
+      <c r="T23" t="n">
+        <v>0.0002620217154741268</v>
+      </c>
+      <c r="U23" t="n">
+        <v>0.0008594046815600682</v>
+      </c>
+      <c r="V23" t="n">
+        <v>3.520126104354858</v>
+      </c>
+      <c r="W23" t="n">
+        <v>4.569626331329346</v>
+      </c>
+      <c r="X23" t="n">
+        <v>2.406062841415405</v>
+      </c>
+      <c r="Y23" t="inlineStr">
+        <is>
+          <t>run with Quantum layer</t>
+        </is>
+      </c>
+      <c r="Z23" t="inlineStr">
+        <is>
+          <t>AAPL, MSFT, GOOGL</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Auto-log: Q=2, D=2, Skip=concat</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>4</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0</v>
+      </c>
+      <c r="F24" t="n">
+        <v>16</v>
+      </c>
+      <c r="G24" t="n">
+        <v>20</v>
+      </c>
+      <c r="H24" t="b">
+        <v>1</v>
+      </c>
+      <c r="I24" t="n">
+        <v>2</v>
+      </c>
+      <c r="J24" t="n">
+        <v>2</v>
+      </c>
+      <c r="K24" t="n">
+        <v>3</v>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>concat</t>
+        </is>
+      </c>
+      <c r="M24" t="inlineStr"/>
+      <c r="N24" t="b">
+        <v>0</v>
+      </c>
+      <c r="O24" t="n">
+        <v>0</v>
+      </c>
+      <c r="P24" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q24" t="inlineStr"/>
+      <c r="R24" t="n">
+        <v>15</v>
+      </c>
+      <c r="S24" t="n">
+        <v>2</v>
+      </c>
+      <c r="T24" t="n">
+        <v>0.0002620220253602577</v>
+      </c>
+      <c r="U24" t="n">
+        <v>0.0008594105707511227</v>
+      </c>
+      <c r="V24" t="n">
+        <v>3.52012825012207</v>
+      </c>
+      <c r="W24" t="n">
+        <v>4.569629192352295</v>
+      </c>
+      <c r="X24" t="n">
+        <v>2.406064748764038</v>
+      </c>
+      <c r="Y24" t="inlineStr">
+        <is>
+          <t>run with Quantum layer</t>
+        </is>
+      </c>
+      <c r="Z24" t="inlineStr">
+        <is>
+          <t>AAPL, MSFT, GOOGL</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Auto-log: Q=2, D=2, Skip=concat</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>4</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0</v>
+      </c>
+      <c r="F25" t="n">
+        <v>16</v>
+      </c>
+      <c r="G25" t="n">
+        <v>20</v>
+      </c>
+      <c r="H25" t="b">
+        <v>1</v>
+      </c>
+      <c r="I25" t="n">
+        <v>2</v>
+      </c>
+      <c r="J25" t="n">
+        <v>2</v>
+      </c>
+      <c r="K25" t="n">
+        <v>3</v>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>concat</t>
+        </is>
+      </c>
+      <c r="M25" t="inlineStr"/>
+      <c r="N25" t="b">
+        <v>0</v>
+      </c>
+      <c r="O25" t="n">
+        <v>0</v>
+      </c>
+      <c r="P25" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q25" t="inlineStr"/>
+      <c r="R25" t="n">
+        <v>15</v>
+      </c>
+      <c r="S25" t="n">
+        <v>2</v>
+      </c>
+      <c r="T25" t="n">
+        <v>0.0002620216280465297</v>
+      </c>
+      <c r="U25" t="n">
+        <v>0.0008594073296990246</v>
+      </c>
+      <c r="V25" t="n">
+        <v>3.520125865936279</v>
+      </c>
+      <c r="W25" t="n">
+        <v>4.569626331329346</v>
+      </c>
+      <c r="X25" t="n">
+        <v>2.406063079833984</v>
+      </c>
+      <c r="Y25" t="inlineStr">
+        <is>
+          <t>test run with Quantum layer</t>
+        </is>
+      </c>
+      <c r="Z25" t="inlineStr">
+        <is>
+          <t>AAPL, MSFT, GOOGL</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
fixed quantum layer not used / classical layer issue
</commit_message>
<xml_diff>
--- a/model/qml_experiment_log.xlsx
+++ b/model/qml_experiment_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Z25"/>
+  <dimension ref="A1:Z27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2503,6 +2503,180 @@
         </is>
       </c>
     </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Auto-log: Q=2, D=2, Skip=concat</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>4</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0</v>
+      </c>
+      <c r="F26" t="n">
+        <v>16</v>
+      </c>
+      <c r="G26" t="n">
+        <v>20</v>
+      </c>
+      <c r="H26" t="b">
+        <v>1</v>
+      </c>
+      <c r="I26" t="n">
+        <v>2</v>
+      </c>
+      <c r="J26" t="n">
+        <v>2</v>
+      </c>
+      <c r="K26" t="n">
+        <v>3</v>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>concat</t>
+        </is>
+      </c>
+      <c r="M26" t="inlineStr"/>
+      <c r="N26" t="b">
+        <v>0</v>
+      </c>
+      <c r="O26" t="n">
+        <v>0</v>
+      </c>
+      <c r="P26" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q26" t="inlineStr"/>
+      <c r="R26" t="n">
+        <v>15</v>
+      </c>
+      <c r="S26" t="n">
+        <v>2</v>
+      </c>
+      <c r="T26" t="n">
+        <v>0.0002126383832875674</v>
+      </c>
+      <c r="U26" t="n">
+        <v>0.0006463956604885096</v>
+      </c>
+      <c r="V26" t="n">
+        <v>3.32081937789917</v>
+      </c>
+      <c r="W26" t="n">
+        <v>4.308806896209717</v>
+      </c>
+      <c r="X26" t="n">
+        <v>2.274315118789673</v>
+      </c>
+      <c r="Y26" t="inlineStr">
+        <is>
+          <t>test run with Quantum layer</t>
+        </is>
+      </c>
+      <c r="Z26" t="inlineStr">
+        <is>
+          <t>AAPL, MSFT, GOOGL</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Auto-log: Q=-, D=-, Skip=concat</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>4</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0</v>
+      </c>
+      <c r="F27" t="n">
+        <v>16</v>
+      </c>
+      <c r="G27" t="n">
+        <v>20</v>
+      </c>
+      <c r="H27" t="b">
+        <v>0</v>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>concat</t>
+        </is>
+      </c>
+      <c r="M27" t="inlineStr"/>
+      <c r="N27" t="b">
+        <v>0</v>
+      </c>
+      <c r="O27" t="n">
+        <v>0</v>
+      </c>
+      <c r="P27" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q27" t="inlineStr"/>
+      <c r="R27" t="n">
+        <v>15</v>
+      </c>
+      <c r="S27" t="n">
+        <v>2</v>
+      </c>
+      <c r="T27" t="n">
+        <v>0.0003715450874300045</v>
+      </c>
+      <c r="U27" t="n">
+        <v>0.007181070270041559</v>
+      </c>
+      <c r="V27" t="n">
+        <v>10.74910068511963</v>
+      </c>
+      <c r="W27" t="n">
+        <v>14.20177745819092</v>
+      </c>
+      <c r="X27" t="n">
+        <v>6.630932331085205</v>
+      </c>
+      <c r="Y27" t="inlineStr">
+        <is>
+          <t>test run with classical only layer</t>
+        </is>
+      </c>
+      <c r="Z27" t="inlineStr">
+        <is>
+          <t>AAPL, MSFT, GOOGL</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
updated model and opt
</commit_message>
<xml_diff>
--- a/model/qml_experiment_log.xlsx
+++ b/model/qml_experiment_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Z28"/>
+  <dimension ref="A1:Z38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -567,11 +567,11 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Auto-log: Q=2, D=2, Skip=concat</t>
+          <t>Auto-log: Q=-, D=-, Skip=concat</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -590,16 +590,22 @@
         <v>20</v>
       </c>
       <c r="H2" t="b">
-        <v>1</v>
-      </c>
-      <c r="I2" t="n">
-        <v>2</v>
-      </c>
-      <c r="J2" t="n">
-        <v>2</v>
-      </c>
-      <c r="K2" t="n">
-        <v>3</v>
+        <v>0</v>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
@@ -611,16 +617,12 @@
         <v>0</v>
       </c>
       <c r="O2" t="n">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="P2" t="b">
         <v>0</v>
       </c>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>Sigmoid</t>
-        </is>
-      </c>
+      <c r="Q2" t="inlineStr"/>
       <c r="R2" t="n">
         <v>5</v>
       </c>
@@ -628,36 +630,36 @@
         <v>2</v>
       </c>
       <c r="T2" t="n">
-        <v>0.002108555850720713</v>
+        <v>0.0002943174301421211</v>
       </c>
       <c r="U2" t="n">
-        <v>0.04601881966664223</v>
+        <v>0.005142642903592787</v>
       </c>
       <c r="V2" t="n">
-        <v>43.08505249023438</v>
+        <v>7.038537502288818</v>
       </c>
       <c r="W2" t="n">
-        <v>49.28862762451172</v>
+        <v>9.478716850280762</v>
       </c>
       <c r="X2" t="inlineStr"/>
       <c r="Y2" t="inlineStr">
         <is>
-          <t>Test on more dynamic data, add dropout and layernorm.</t>
+          <t>Classical Run with LSTM, no dropout, no layernorm, no quantum layer</t>
         </is>
       </c>
       <c r="Z2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Auto-log: Q=2, D=2, Skip=concat</t>
+          <t>Auto-log: Q=-, D=-, Skip=concat</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
@@ -672,16 +674,22 @@
         <v>20</v>
       </c>
       <c r="H3" t="b">
-        <v>1</v>
-      </c>
-      <c r="I3" t="n">
-        <v>2</v>
-      </c>
-      <c r="J3" t="n">
-        <v>2</v>
-      </c>
-      <c r="K3" t="n">
-        <v>3</v>
+        <v>0</v>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
@@ -700,34 +708,40 @@
       </c>
       <c r="Q3" t="inlineStr"/>
       <c r="R3" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="S3" t="n">
         <v>2</v>
       </c>
       <c r="T3" t="n">
-        <v>0.0003446844676213842</v>
+        <v>0.0003715450874300045</v>
       </c>
       <c r="U3" t="n">
-        <v>0.009985854365368141</v>
+        <v>0.007181070270041559</v>
       </c>
       <c r="V3" t="n">
-        <v>9.179535865783691</v>
+        <v>10.74910068511963</v>
       </c>
       <c r="W3" t="n">
-        <v>12.9601879119873</v>
-      </c>
-      <c r="X3" t="inlineStr"/>
+        <v>14.20177745819092</v>
+      </c>
+      <c r="X3" t="n">
+        <v>6.630932331085205</v>
+      </c>
       <c r="Y3" t="inlineStr">
         <is>
-          <t>Test on more dynamic data, add dropout and layernorm.</t>
-        </is>
-      </c>
-      <c r="Z3" t="inlineStr"/>
+          <t>test run with classical only layer</t>
+        </is>
+      </c>
+      <c r="Z3" t="inlineStr">
+        <is>
+          <t>AAPL, MSFT, GOOGL</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -771,12 +785,16 @@
         <v>0</v>
       </c>
       <c r="O4" t="n">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="P4" t="b">
         <v>0</v>
       </c>
-      <c r="Q4" t="inlineStr"/>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>Sigmoid</t>
+        </is>
+      </c>
       <c r="R4" t="n">
         <v>5</v>
       </c>
@@ -784,24 +802,28 @@
         <v>2</v>
       </c>
       <c r="T4" t="n">
-        <v>0.0002545558669399249</v>
+        <v>0.002108555850720713</v>
       </c>
       <c r="U4" t="n">
-        <v>0.009765016884557554</v>
+        <v>0.04601881966664223</v>
       </c>
       <c r="V4" t="n">
-        <v>17.51806831359863</v>
+        <v>43.08505249023438</v>
       </c>
       <c r="W4" t="n">
-        <v>22.26754760742188</v>
+        <v>49.28862762451172</v>
       </c>
       <c r="X4" t="inlineStr"/>
-      <c r="Y4" t="inlineStr"/>
+      <c r="Y4" t="inlineStr">
+        <is>
+          <t>Test on more dynamic data, add dropout and layernorm.</t>
+        </is>
+      </c>
       <c r="Z4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -858,28 +880,32 @@
         <v>2</v>
       </c>
       <c r="T5" t="n">
-        <v>0.0004298115511321359</v>
+        <v>0.0003446844676213842</v>
       </c>
       <c r="U5" t="n">
-        <v>0.01697197027715447</v>
+        <v>0.009985854365368141</v>
       </c>
       <c r="V5" t="n">
-        <v>23.2319278717041</v>
+        <v>9.179535865783691</v>
       </c>
       <c r="W5" t="n">
-        <v>29.44417381286621</v>
+        <v>12.9601879119873</v>
       </c>
       <c r="X5" t="inlineStr"/>
-      <c r="Y5" t="inlineStr"/>
+      <c r="Y5" t="inlineStr">
+        <is>
+          <t>Test on more dynamic data, add dropout and layernorm.</t>
+        </is>
+      </c>
       <c r="Z5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Auto-log: Q=-, D=-, Skip=concat</t>
+          <t>Auto-log: Q=2, D=2, Skip=concat</t>
         </is>
       </c>
       <c r="C6" t="n">
@@ -898,22 +924,16 @@
         <v>20</v>
       </c>
       <c r="H6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+        <v>1</v>
+      </c>
+      <c r="I6" t="n">
+        <v>2</v>
+      </c>
+      <c r="J6" t="n">
+        <v>2</v>
+      </c>
+      <c r="K6" t="n">
+        <v>3</v>
       </c>
       <c r="L6" t="inlineStr">
         <is>
@@ -938,28 +958,24 @@
         <v>2</v>
       </c>
       <c r="T6" t="n">
-        <v>0.0002943174301421211</v>
+        <v>0.0002545558669399249</v>
       </c>
       <c r="U6" t="n">
-        <v>0.005142642903592787</v>
+        <v>0.009765016884557554</v>
       </c>
       <c r="V6" t="n">
-        <v>7.038537502288818</v>
+        <v>17.51806831359863</v>
       </c>
       <c r="W6" t="n">
-        <v>9.478716850280762</v>
+        <v>22.26754760742188</v>
       </c>
       <c r="X6" t="inlineStr"/>
-      <c r="Y6" t="inlineStr">
-        <is>
-          <t>Classical Run with LSTM, no dropout, no layernorm, no quantum layer</t>
-        </is>
-      </c>
+      <c r="Y6" t="inlineStr"/>
       <c r="Z6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -1016,28 +1032,24 @@
         <v>2</v>
       </c>
       <c r="T7" t="n">
-        <v>0.00104064371119002</v>
+        <v>0.0004298115511321359</v>
       </c>
       <c r="U7" t="n">
-        <v>0.03594797892583301</v>
+        <v>0.01697197027715447</v>
       </c>
       <c r="V7" t="n">
-        <v>36.3784065246582</v>
+        <v>23.2319278717041</v>
       </c>
       <c r="W7" t="n">
-        <v>43.2968635559082</v>
+        <v>29.44417381286621</v>
       </c>
       <c r="X7" t="inlineStr"/>
-      <c r="Y7" t="inlineStr">
-        <is>
-          <t>run with Quantum layer</t>
-        </is>
-      </c>
+      <c r="Y7" t="inlineStr"/>
       <c r="Z7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -1094,16 +1106,16 @@
         <v>2</v>
       </c>
       <c r="T8" t="n">
-        <v>0.0004212268501601463</v>
+        <v>0.00104064371119002</v>
       </c>
       <c r="U8" t="n">
-        <v>0.01748553632569383</v>
+        <v>0.03594797892583301</v>
       </c>
       <c r="V8" t="n">
-        <v>24.41910552978516</v>
+        <v>36.3784065246582</v>
       </c>
       <c r="W8" t="n">
-        <v>30.00810432434082</v>
+        <v>43.2968635559082</v>
       </c>
       <c r="X8" t="inlineStr"/>
       <c r="Y8" t="inlineStr">
@@ -1115,7 +1127,7 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -1172,10 +1184,10 @@
         <v>2</v>
       </c>
       <c r="T9" t="n">
-        <v>0.0004212268776470973</v>
+        <v>0.0004212268501601463</v>
       </c>
       <c r="U9" t="n">
-        <v>0.01748553487777826</v>
+        <v>0.01748553632569383</v>
       </c>
       <c r="V9" t="n">
         <v>24.41910552978516</v>
@@ -1193,7 +1205,7 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -1250,20 +1262,18 @@
         <v>2</v>
       </c>
       <c r="T10" t="n">
-        <v>0.0004212267852539847</v>
+        <v>0.0004212268776470973</v>
       </c>
       <c r="U10" t="n">
-        <v>0.01748553015568177</v>
+        <v>0.01748553487777826</v>
       </c>
       <c r="V10" t="n">
-        <v>24.41909980773926</v>
+        <v>24.41910552978516</v>
       </c>
       <c r="W10" t="n">
-        <v>30.00810050964355</v>
-      </c>
-      <c r="X10" t="n">
-        <v>11.91269683837891</v>
-      </c>
+        <v>30.00810432434082</v>
+      </c>
+      <c r="X10" t="inlineStr"/>
       <c r="Y10" t="inlineStr">
         <is>
           <t>run with Quantum layer</t>
@@ -1273,7 +1283,7 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -1284,7 +1294,7 @@
         <v>1</v>
       </c>
       <c r="D11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11" t="n">
         <v>0</v>
@@ -1330,19 +1340,19 @@
         <v>2</v>
       </c>
       <c r="T11" t="n">
-        <v>0.0004659449900611348</v>
+        <v>0.0004212267852539847</v>
       </c>
       <c r="U11" t="n">
-        <v>0.01726520269585308</v>
+        <v>0.01748553015568177</v>
       </c>
       <c r="V11" t="n">
-        <v>23.11555099487305</v>
+        <v>24.41909980773926</v>
       </c>
       <c r="W11" t="n">
-        <v>29.64953231811523</v>
+        <v>30.00810050964355</v>
       </c>
       <c r="X11" t="n">
-        <v>11.15723609924316</v>
+        <v>11.91269683837891</v>
       </c>
       <c r="Y11" t="inlineStr">
         <is>
@@ -1353,7 +1363,7 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -1361,7 +1371,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D12" t="n">
         <v>1</v>
@@ -1404,25 +1414,25 @@
       </c>
       <c r="Q12" t="inlineStr"/>
       <c r="R12" t="n">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="S12" t="n">
         <v>2</v>
       </c>
       <c r="T12" t="n">
-        <v>0.0002755922186123725</v>
+        <v>0.0004659449900611348</v>
       </c>
       <c r="U12" t="n">
-        <v>0.008164557970303576</v>
+        <v>0.01726520269585308</v>
       </c>
       <c r="V12" t="n">
-        <v>14.92195510864258</v>
+        <v>23.11555099487305</v>
       </c>
       <c r="W12" t="n">
-        <v>19.71026420593262</v>
+        <v>29.64953231811523</v>
       </c>
       <c r="X12" t="n">
-        <v>7.186328411102295</v>
+        <v>11.15723609924316</v>
       </c>
       <c r="Y12" t="inlineStr">
         <is>
@@ -1433,7 +1443,7 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -1444,7 +1454,7 @@
         <v>2</v>
       </c>
       <c r="D13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
@@ -1490,19 +1500,19 @@
         <v>2</v>
       </c>
       <c r="T13" t="n">
-        <v>0.0002311510873527917</v>
+        <v>0.0002755922186123725</v>
       </c>
       <c r="U13" t="n">
-        <v>0.006108876623329706</v>
+        <v>0.008164557970303576</v>
       </c>
       <c r="V13" t="n">
-        <v>12.91889095306396</v>
+        <v>14.92195510864258</v>
       </c>
       <c r="W13" t="n">
-        <v>17.25859451293945</v>
+        <v>19.71026420593262</v>
       </c>
       <c r="X13" t="n">
-        <v>6.20987606048584</v>
+        <v>7.186328411102295</v>
       </c>
       <c r="Y13" t="inlineStr">
         <is>
@@ -1513,7 +1523,7 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -1521,7 +1531,7 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D14" t="n">
         <v>0</v>
@@ -1570,19 +1580,19 @@
         <v>2</v>
       </c>
       <c r="T14" t="n">
-        <v>0.0006707275329279669</v>
+        <v>0.0002311510873527917</v>
       </c>
       <c r="U14" t="n">
-        <v>0.01115978131565498</v>
+        <v>0.006108876623329706</v>
       </c>
       <c r="V14" t="n">
-        <v>15.28087520599365</v>
+        <v>12.91889095306396</v>
       </c>
       <c r="W14" t="n">
-        <v>21.42845153808594</v>
+        <v>17.25859451293945</v>
       </c>
       <c r="X14" t="n">
-        <v>7.279820442199707</v>
+        <v>6.20987606048584</v>
       </c>
       <c r="Y14" t="inlineStr">
         <is>
@@ -1593,7 +1603,7 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -1650,19 +1660,19 @@
         <v>2</v>
       </c>
       <c r="T15" t="n">
-        <v>1.132239412982017e-05</v>
+        <v>0.0006707275329279669</v>
       </c>
       <c r="U15" t="n">
-        <v>5.341193536878563e-05</v>
+        <v>0.01115978131565498</v>
       </c>
       <c r="V15" t="n">
-        <v>0.1708307266235352</v>
+        <v>15.28087520599365</v>
       </c>
       <c r="W15" t="n">
-        <v>0.1843285113573074</v>
+        <v>21.42845153808594</v>
       </c>
       <c r="X15" t="n">
-        <v>0.60400390625</v>
+        <v>7.279820442199707</v>
       </c>
       <c r="Y15" t="inlineStr">
         <is>
@@ -1673,7 +1683,7 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -1730,19 +1740,19 @@
         <v>2</v>
       </c>
       <c r="T16" t="n">
-        <v>0.0006707280517152939</v>
+        <v>1.132239412982017e-05</v>
       </c>
       <c r="U16" t="n">
-        <v>0.01115977805784496</v>
+        <v>5.341193536878563e-05</v>
       </c>
       <c r="V16" t="n">
-        <v>15.28087711334229</v>
+        <v>0.1708307266235352</v>
       </c>
       <c r="W16" t="n">
-        <v>21.42845344543457</v>
+        <v>0.1843285113573074</v>
       </c>
       <c r="X16" t="n">
-        <v>7.279821395874023</v>
+        <v>0.60400390625</v>
       </c>
       <c r="Y16" t="inlineStr">
         <is>
@@ -1753,7 +1763,7 @@
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -1810,19 +1820,19 @@
         <v>2</v>
       </c>
       <c r="T17" t="n">
-        <v>0.0002620218473702095</v>
+        <v>0.0006707280517152939</v>
       </c>
       <c r="U17" t="n">
-        <v>0.0008594085127387711</v>
+        <v>0.01115977805784496</v>
       </c>
       <c r="V17" t="n">
-        <v>3.520127534866333</v>
+        <v>15.28087711334229</v>
       </c>
       <c r="W17" t="n">
-        <v>4.569629192352295</v>
+        <v>21.42845344543457</v>
       </c>
       <c r="X17" t="n">
-        <v>2.406062841415405</v>
+        <v>7.279821395874023</v>
       </c>
       <c r="Y17" t="inlineStr">
         <is>
@@ -1833,7 +1843,7 @@
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -1906,18 +1916,14 @@
       </c>
       <c r="Y18" t="inlineStr">
         <is>
-          <t>Multi-ticker experiment with LSTM+Quantum</t>
-        </is>
-      </c>
-      <c r="Z18" t="inlineStr">
-        <is>
-          <t>AAPL, MSFT, GOOGL</t>
-        </is>
-      </c>
+          <t>run with Quantum layer</t>
+        </is>
+      </c>
+      <c r="Z18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -1990,7 +1996,7 @@
       </c>
       <c r="Y19" t="inlineStr">
         <is>
-          <t>run with Quantum layer</t>
+          <t>Multi-ticker experiment with LSTM+Quantum</t>
         </is>
       </c>
       <c r="Z19" t="inlineStr">
@@ -2001,7 +2007,7 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
@@ -2058,19 +2064,19 @@
         <v>2</v>
       </c>
       <c r="T20" t="n">
-        <v>0.0002620216811455395</v>
+        <v>0.0002620218473702095</v>
       </c>
       <c r="U20" t="n">
-        <v>0.0008594098481092047</v>
+        <v>0.0008594085127387711</v>
       </c>
       <c r="V20" t="n">
         <v>3.520127534866333</v>
       </c>
       <c r="W20" t="n">
-        <v>4.569628238677979</v>
+        <v>4.569629192352295</v>
       </c>
       <c r="X20" t="n">
-        <v>2.406063079833984</v>
+        <v>2.406062841415405</v>
       </c>
       <c r="Y20" t="inlineStr">
         <is>
@@ -2085,7 +2091,7 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
@@ -2142,10 +2148,10 @@
         <v>2</v>
       </c>
       <c r="T21" t="n">
-        <v>0.0002620218950122511</v>
+        <v>0.0002620216811455395</v>
       </c>
       <c r="U21" t="n">
-        <v>0.0008594071114202961</v>
+        <v>0.0008594098481092047</v>
       </c>
       <c r="V21" t="n">
         <v>3.520127534866333</v>
@@ -2154,7 +2160,7 @@
         <v>4.569628238677979</v>
       </c>
       <c r="X21" t="n">
-        <v>2.40606427192688</v>
+        <v>2.406063079833984</v>
       </c>
       <c r="Y21" t="inlineStr">
         <is>
@@ -2169,7 +2175,7 @@
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
@@ -2226,13 +2232,13 @@
         <v>2</v>
       </c>
       <c r="T22" t="n">
-        <v>0.0002620217367988749</v>
+        <v>0.0002620218950122511</v>
       </c>
       <c r="U22" t="n">
-        <v>0.00085940357437605</v>
+        <v>0.0008594071114202961</v>
       </c>
       <c r="V22" t="n">
-        <v>3.520126819610596</v>
+        <v>3.520127534866333</v>
       </c>
       <c r="W22" t="n">
         <v>4.569628238677979</v>
@@ -2253,7 +2259,7 @@
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
@@ -2310,19 +2316,19 @@
         <v>2</v>
       </c>
       <c r="T23" t="n">
-        <v>0.0002620217154741268</v>
+        <v>0.0002620217367988749</v>
       </c>
       <c r="U23" t="n">
-        <v>0.0008594046815600682</v>
+        <v>0.00085940357437605</v>
       </c>
       <c r="V23" t="n">
-        <v>3.520126104354858</v>
+        <v>3.520126819610596</v>
       </c>
       <c r="W23" t="n">
-        <v>4.569626331329346</v>
+        <v>4.569628238677979</v>
       </c>
       <c r="X23" t="n">
-        <v>2.406062841415405</v>
+        <v>2.40606427192688</v>
       </c>
       <c r="Y23" t="inlineStr">
         <is>
@@ -2337,7 +2343,7 @@
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
@@ -2394,19 +2400,19 @@
         <v>2</v>
       </c>
       <c r="T24" t="n">
-        <v>0.0002620220253602577</v>
+        <v>0.0002620217154741268</v>
       </c>
       <c r="U24" t="n">
-        <v>0.0008594105707511227</v>
+        <v>0.0008594046815600682</v>
       </c>
       <c r="V24" t="n">
-        <v>3.52012825012207</v>
+        <v>3.520126104354858</v>
       </c>
       <c r="W24" t="n">
-        <v>4.569629192352295</v>
+        <v>4.569626331329346</v>
       </c>
       <c r="X24" t="n">
-        <v>2.406064748764038</v>
+        <v>2.406062841415405</v>
       </c>
       <c r="Y24" t="inlineStr">
         <is>
@@ -2421,7 +2427,7 @@
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
@@ -2478,23 +2484,23 @@
         <v>2</v>
       </c>
       <c r="T25" t="n">
-        <v>0.0002620216280465297</v>
+        <v>0.0002620220253602577</v>
       </c>
       <c r="U25" t="n">
-        <v>0.0008594073296990246</v>
+        <v>0.0008594105707511227</v>
       </c>
       <c r="V25" t="n">
-        <v>3.520125865936279</v>
+        <v>3.52012825012207</v>
       </c>
       <c r="W25" t="n">
-        <v>4.569626331329346</v>
+        <v>4.569629192352295</v>
       </c>
       <c r="X25" t="n">
-        <v>2.406063079833984</v>
+        <v>2.406064748764038</v>
       </c>
       <c r="Y25" t="inlineStr">
         <is>
-          <t>test run with Quantum layer</t>
+          <t>run with Quantum layer</t>
         </is>
       </c>
       <c r="Z25" t="inlineStr">
@@ -2505,7 +2511,7 @@
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
@@ -2562,19 +2568,19 @@
         <v>2</v>
       </c>
       <c r="T26" t="n">
-        <v>0.0002126383832875674</v>
+        <v>0.0002620216280465297</v>
       </c>
       <c r="U26" t="n">
-        <v>0.0006463956604885096</v>
+        <v>0.0008594073296990246</v>
       </c>
       <c r="V26" t="n">
-        <v>3.32081937789917</v>
+        <v>3.520125865936279</v>
       </c>
       <c r="W26" t="n">
-        <v>4.308806896209717</v>
+        <v>4.569626331329346</v>
       </c>
       <c r="X26" t="n">
-        <v>2.274315118789673</v>
+        <v>2.406063079833984</v>
       </c>
       <c r="Y26" t="inlineStr">
         <is>
@@ -2589,11 +2595,11 @@
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Auto-log: Q=-, D=-, Skip=concat</t>
+          <t>Auto-log: Q=2, D=2, Skip=concat</t>
         </is>
       </c>
       <c r="C27" t="n">
@@ -2612,22 +2618,16 @@
         <v>20</v>
       </c>
       <c r="H27" t="b">
-        <v>0</v>
-      </c>
-      <c r="I27" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="J27" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K27" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+        <v>1</v>
+      </c>
+      <c r="I27" t="n">
+        <v>2</v>
+      </c>
+      <c r="J27" t="n">
+        <v>2</v>
+      </c>
+      <c r="K27" t="n">
+        <v>3</v>
       </c>
       <c r="L27" t="inlineStr">
         <is>
@@ -2652,23 +2652,23 @@
         <v>2</v>
       </c>
       <c r="T27" t="n">
-        <v>0.0003715450874300045</v>
+        <v>0.0002126383832875674</v>
       </c>
       <c r="U27" t="n">
-        <v>0.007181070270041559</v>
+        <v>0.0006463956604885096</v>
       </c>
       <c r="V27" t="n">
-        <v>10.74910068511963</v>
+        <v>3.32081937789917</v>
       </c>
       <c r="W27" t="n">
-        <v>14.20177745819092</v>
+        <v>4.308806896209717</v>
       </c>
       <c r="X27" t="n">
-        <v>6.630932331085205</v>
+        <v>2.274315118789673</v>
       </c>
       <c r="Y27" t="inlineStr">
         <is>
-          <t>test run with classical only layer</t>
+          <t>test run with Quantum layer</t>
         </is>
       </c>
       <c r="Z27" t="inlineStr">
@@ -2756,6 +2756,866 @@
         </is>
       </c>
       <c r="Z28" t="inlineStr">
+        <is>
+          <t>AAPL, MSFT, GOOGL</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Auto-log: Q=6, D=4, Skip=concat</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>0</v>
+      </c>
+      <c r="D29" t="n">
+        <v>4</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0</v>
+      </c>
+      <c r="F29" t="n">
+        <v>32</v>
+      </c>
+      <c r="G29" t="n">
+        <v>20</v>
+      </c>
+      <c r="H29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I29" t="n">
+        <v>6</v>
+      </c>
+      <c r="J29" t="n">
+        <v>4</v>
+      </c>
+      <c r="K29" t="n">
+        <v>3</v>
+      </c>
+      <c r="L29" t="inlineStr">
+        <is>
+          <t>concat</t>
+        </is>
+      </c>
+      <c r="M29" t="inlineStr"/>
+      <c r="N29" t="b">
+        <v>0</v>
+      </c>
+      <c r="O29" t="n">
+        <v>0</v>
+      </c>
+      <c r="P29" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q29" t="inlineStr"/>
+      <c r="R29" t="n">
+        <v>10</v>
+      </c>
+      <c r="S29" t="n">
+        <v>2</v>
+      </c>
+      <c r="T29" t="n">
+        <v>0.0001274058098560806</v>
+      </c>
+      <c r="U29" t="n">
+        <v>0.001787280394792299</v>
+      </c>
+      <c r="V29" t="n">
+        <v>5.124116897583008</v>
+      </c>
+      <c r="W29" t="n">
+        <v>7.182210922241211</v>
+      </c>
+      <c r="X29" t="n">
+        <v>3.169698238372803</v>
+      </c>
+      <c r="Y29" t="inlineStr">
+        <is>
+          <t>test run with classical only layer</t>
+        </is>
+      </c>
+      <c r="Z29" t="inlineStr">
+        <is>
+          <t>AAPL, MSFT, GOOGL</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Auto-log: Q=6, D=4, Skip=add</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>0</v>
+      </c>
+      <c r="D30" t="n">
+        <v>2</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0</v>
+      </c>
+      <c r="F30" t="n">
+        <v>32</v>
+      </c>
+      <c r="G30" t="n">
+        <v>20</v>
+      </c>
+      <c r="H30" t="b">
+        <v>1</v>
+      </c>
+      <c r="I30" t="n">
+        <v>6</v>
+      </c>
+      <c r="J30" t="n">
+        <v>4</v>
+      </c>
+      <c r="K30" t="n">
+        <v>3</v>
+      </c>
+      <c r="L30" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="M30" t="inlineStr">
+        <is>
+          <t>Tanh</t>
+        </is>
+      </c>
+      <c r="N30" t="b">
+        <v>0</v>
+      </c>
+      <c r="O30" t="n">
+        <v>0</v>
+      </c>
+      <c r="P30" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q30" t="inlineStr"/>
+      <c r="R30" t="n">
+        <v>10</v>
+      </c>
+      <c r="S30" t="n">
+        <v>2</v>
+      </c>
+      <c r="T30" t="n">
+        <v>0.0001256674930970048</v>
+      </c>
+      <c r="U30" t="n">
+        <v>0.0009276028499601686</v>
+      </c>
+      <c r="V30" t="n">
+        <v>3.828903675079346</v>
+      </c>
+      <c r="W30" t="n">
+        <v>4.949349880218506</v>
+      </c>
+      <c r="X30" t="n">
+        <v>2.484735012054443</v>
+      </c>
+      <c r="Y30" t="inlineStr">
+        <is>
+          <t>test run with classical only layer</t>
+        </is>
+      </c>
+      <c r="Z30" t="inlineStr">
+        <is>
+          <t>AAPL, MSFT, GOOGL</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Auto-log: Q=6, D=4, Skip=add</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>0</v>
+      </c>
+      <c r="D31" t="n">
+        <v>2</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0</v>
+      </c>
+      <c r="F31" t="n">
+        <v>32</v>
+      </c>
+      <c r="G31" t="n">
+        <v>20</v>
+      </c>
+      <c r="H31" t="b">
+        <v>1</v>
+      </c>
+      <c r="I31" t="n">
+        <v>6</v>
+      </c>
+      <c r="J31" t="n">
+        <v>4</v>
+      </c>
+      <c r="K31" t="n">
+        <v>3</v>
+      </c>
+      <c r="L31" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="M31" t="inlineStr">
+        <is>
+          <t>Tanh</t>
+        </is>
+      </c>
+      <c r="N31" t="b">
+        <v>0</v>
+      </c>
+      <c r="O31" t="n">
+        <v>0</v>
+      </c>
+      <c r="P31" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q31" t="inlineStr"/>
+      <c r="R31" t="n">
+        <v>20</v>
+      </c>
+      <c r="S31" t="n">
+        <v>4</v>
+      </c>
+      <c r="T31" t="n">
+        <v>0.0001095112613276139</v>
+      </c>
+      <c r="U31" t="n">
+        <v>0.001054700336139154</v>
+      </c>
+      <c r="V31" t="n">
+        <v>3.828903675079346</v>
+      </c>
+      <c r="W31" t="n">
+        <v>4.949349880218506</v>
+      </c>
+      <c r="X31" t="n">
+        <v>2.484735012054443</v>
+      </c>
+      <c r="Y31" t="inlineStr">
+        <is>
+          <t>test run with classical only layer</t>
+        </is>
+      </c>
+      <c r="Z31" t="inlineStr">
+        <is>
+          <t>AAPL, MSFT, GOOGL</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Auto-log: Q=6, D=4, Skip=add</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>0</v>
+      </c>
+      <c r="D32" t="n">
+        <v>4</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0</v>
+      </c>
+      <c r="F32" t="n">
+        <v>32</v>
+      </c>
+      <c r="G32" t="n">
+        <v>20</v>
+      </c>
+      <c r="H32" t="b">
+        <v>1</v>
+      </c>
+      <c r="I32" t="n">
+        <v>6</v>
+      </c>
+      <c r="J32" t="n">
+        <v>4</v>
+      </c>
+      <c r="K32" t="n">
+        <v>3</v>
+      </c>
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="M32" t="inlineStr">
+        <is>
+          <t>Tanh</t>
+        </is>
+      </c>
+      <c r="N32" t="b">
+        <v>0</v>
+      </c>
+      <c r="O32" t="n">
+        <v>0</v>
+      </c>
+      <c r="P32" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q32" t="inlineStr"/>
+      <c r="R32" t="n">
+        <v>20</v>
+      </c>
+      <c r="S32" t="n">
+        <v>4</v>
+      </c>
+      <c r="T32" t="n">
+        <v>9.676977778655511e-05</v>
+      </c>
+      <c r="U32" t="n">
+        <v>0.001749778865524469</v>
+      </c>
+      <c r="V32" t="n">
+        <v>3.640385866165161</v>
+      </c>
+      <c r="W32" t="n">
+        <v>4.423428535461426</v>
+      </c>
+      <c r="X32" t="n">
+        <v>2.494111299514771</v>
+      </c>
+      <c r="Y32" t="inlineStr">
+        <is>
+          <t>test run with classical only layer</t>
+        </is>
+      </c>
+      <c r="Z32" t="inlineStr">
+        <is>
+          <t>AAPL, MSFT, GOOGL</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Auto-log: Q=2, D=2, Skip=concat</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>4</v>
+      </c>
+      <c r="D33" t="n">
+        <v>0</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0</v>
+      </c>
+      <c r="F33" t="n">
+        <v>32</v>
+      </c>
+      <c r="G33" t="n">
+        <v>20</v>
+      </c>
+      <c r="H33" t="b">
+        <v>1</v>
+      </c>
+      <c r="I33" t="n">
+        <v>2</v>
+      </c>
+      <c r="J33" t="n">
+        <v>2</v>
+      </c>
+      <c r="K33" t="n">
+        <v>3</v>
+      </c>
+      <c r="L33" t="inlineStr">
+        <is>
+          <t>concat</t>
+        </is>
+      </c>
+      <c r="M33" t="inlineStr"/>
+      <c r="N33" t="b">
+        <v>0</v>
+      </c>
+      <c r="O33" t="n">
+        <v>0</v>
+      </c>
+      <c r="P33" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q33" t="inlineStr"/>
+      <c r="R33" t="n">
+        <v>20</v>
+      </c>
+      <c r="S33" t="n">
+        <v>2</v>
+      </c>
+      <c r="T33" t="n">
+        <v>0.0002189911191093647</v>
+      </c>
+      <c r="U33" t="n">
+        <v>0.001547478709402098</v>
+      </c>
+      <c r="V33" t="n">
+        <v>4.422037601470947</v>
+      </c>
+      <c r="W33" t="n">
+        <v>5.751986980438232</v>
+      </c>
+      <c r="X33" t="n">
+        <v>2.966715097427368</v>
+      </c>
+      <c r="Y33" t="inlineStr">
+        <is>
+          <t>test run with classical only layer</t>
+        </is>
+      </c>
+      <c r="Z33" t="inlineStr">
+        <is>
+          <t>AAPL, MSFT, GOOGL</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Auto-log: Q=2, D=2, Skip=add</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>0</v>
+      </c>
+      <c r="D34" t="n">
+        <v>4</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0</v>
+      </c>
+      <c r="F34" t="n">
+        <v>32</v>
+      </c>
+      <c r="G34" t="n">
+        <v>20</v>
+      </c>
+      <c r="H34" t="b">
+        <v>1</v>
+      </c>
+      <c r="I34" t="n">
+        <v>2</v>
+      </c>
+      <c r="J34" t="n">
+        <v>2</v>
+      </c>
+      <c r="K34" t="n">
+        <v>3</v>
+      </c>
+      <c r="L34" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="M34" t="inlineStr"/>
+      <c r="N34" t="b">
+        <v>0</v>
+      </c>
+      <c r="O34" t="n">
+        <v>0</v>
+      </c>
+      <c r="P34" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q34" t="inlineStr"/>
+      <c r="R34" t="n">
+        <v>20</v>
+      </c>
+      <c r="S34" t="n">
+        <v>2</v>
+      </c>
+      <c r="T34" t="n">
+        <v>0.00012697648756262</v>
+      </c>
+      <c r="U34" t="n">
+        <v>0.001084551319047719</v>
+      </c>
+      <c r="V34" t="n">
+        <v>4.095373630523682</v>
+      </c>
+      <c r="W34" t="n">
+        <v>5.391138076782227</v>
+      </c>
+      <c r="X34" t="n">
+        <v>2.622022867202759</v>
+      </c>
+      <c r="Y34" t="inlineStr">
+        <is>
+          <t>test run with classical only layer</t>
+        </is>
+      </c>
+      <c r="Z34" t="inlineStr">
+        <is>
+          <t>AAPL, MSFT, GOOGL</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Auto-log: Q=2, D=2, Skip=add</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>0</v>
+      </c>
+      <c r="D35" t="n">
+        <v>4</v>
+      </c>
+      <c r="E35" t="n">
+        <v>0</v>
+      </c>
+      <c r="F35" t="n">
+        <v>16</v>
+      </c>
+      <c r="G35" t="n">
+        <v>20</v>
+      </c>
+      <c r="H35" t="b">
+        <v>1</v>
+      </c>
+      <c r="I35" t="n">
+        <v>2</v>
+      </c>
+      <c r="J35" t="n">
+        <v>2</v>
+      </c>
+      <c r="K35" t="n">
+        <v>3</v>
+      </c>
+      <c r="L35" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="M35" t="inlineStr"/>
+      <c r="N35" t="b">
+        <v>0</v>
+      </c>
+      <c r="O35" t="n">
+        <v>0</v>
+      </c>
+      <c r="P35" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q35" t="inlineStr"/>
+      <c r="R35" t="n">
+        <v>20</v>
+      </c>
+      <c r="S35" t="n">
+        <v>2</v>
+      </c>
+      <c r="T35" t="n">
+        <v>0.0001193417208807969</v>
+      </c>
+      <c r="U35" t="n">
+        <v>0.002039353551461976</v>
+      </c>
+      <c r="V35" t="n">
+        <v>5.25993537902832</v>
+      </c>
+      <c r="W35" t="n">
+        <v>7.151086330413818</v>
+      </c>
+      <c r="X35" t="n">
+        <v>3.250463485717773</v>
+      </c>
+      <c r="Y35" t="inlineStr">
+        <is>
+          <t>test run with classical only layer</t>
+        </is>
+      </c>
+      <c r="Z35" t="inlineStr">
+        <is>
+          <t>AAPL, MSFT, GOOGL</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Auto-log: Q=6, D=4, Skip=add</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>0</v>
+      </c>
+      <c r="D36" t="n">
+        <v>4</v>
+      </c>
+      <c r="E36" t="n">
+        <v>0</v>
+      </c>
+      <c r="F36" t="n">
+        <v>32</v>
+      </c>
+      <c r="G36" t="n">
+        <v>20</v>
+      </c>
+      <c r="H36" t="b">
+        <v>1</v>
+      </c>
+      <c r="I36" t="n">
+        <v>6</v>
+      </c>
+      <c r="J36" t="n">
+        <v>4</v>
+      </c>
+      <c r="K36" t="n">
+        <v>3</v>
+      </c>
+      <c r="L36" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="M36" t="inlineStr"/>
+      <c r="N36" t="b">
+        <v>0</v>
+      </c>
+      <c r="O36" t="n">
+        <v>0</v>
+      </c>
+      <c r="P36" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q36" t="inlineStr"/>
+      <c r="R36" t="n">
+        <v>20</v>
+      </c>
+      <c r="S36" t="n">
+        <v>3</v>
+      </c>
+      <c r="T36" t="n">
+        <v>0.0001624533628312341</v>
+      </c>
+      <c r="U36" t="n">
+        <v>0.002016121583515184</v>
+      </c>
+      <c r="V36" t="n">
+        <v>5.616809368133545</v>
+      </c>
+      <c r="W36" t="n">
+        <v>7.522606372833252</v>
+      </c>
+      <c r="X36" t="n">
+        <v>3.511857748031616</v>
+      </c>
+      <c r="Y36" t="inlineStr">
+        <is>
+          <t>test run with classical only layer</t>
+        </is>
+      </c>
+      <c r="Z36" t="inlineStr">
+        <is>
+          <t>AAPL, MSFT, GOOGL</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Auto-log: Q=6, D=4, Skip=add</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>0</v>
+      </c>
+      <c r="D37" t="n">
+        <v>4</v>
+      </c>
+      <c r="E37" t="n">
+        <v>0</v>
+      </c>
+      <c r="F37" t="n">
+        <v>32</v>
+      </c>
+      <c r="G37" t="n">
+        <v>20</v>
+      </c>
+      <c r="H37" t="b">
+        <v>1</v>
+      </c>
+      <c r="I37" t="n">
+        <v>6</v>
+      </c>
+      <c r="J37" t="n">
+        <v>4</v>
+      </c>
+      <c r="K37" t="n">
+        <v>3</v>
+      </c>
+      <c r="L37" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="M37" t="inlineStr">
+        <is>
+          <t>Tanh</t>
+        </is>
+      </c>
+      <c r="N37" t="b">
+        <v>1</v>
+      </c>
+      <c r="O37" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="P37" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q37" t="inlineStr"/>
+      <c r="R37" t="n">
+        <v>20</v>
+      </c>
+      <c r="S37" t="n">
+        <v>4</v>
+      </c>
+      <c r="T37" t="n">
+        <v>0.0001648213271263113</v>
+      </c>
+      <c r="U37" t="n">
+        <v>0.002773941670076307</v>
+      </c>
+      <c r="V37" t="n">
+        <v>4.760529041290283</v>
+      </c>
+      <c r="W37" t="n">
+        <v>6.495021820068359</v>
+      </c>
+      <c r="X37" t="n">
+        <v>2.998628854751587</v>
+      </c>
+      <c r="Y37" t="inlineStr">
+        <is>
+          <t>test run with classical only layer</t>
+        </is>
+      </c>
+      <c r="Z37" t="inlineStr">
+        <is>
+          <t>AAPL, MSFT, GOOGL</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Auto-log: Q=6, D=4, Skip=add</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>0</v>
+      </c>
+      <c r="D38" t="n">
+        <v>4</v>
+      </c>
+      <c r="E38" t="n">
+        <v>0</v>
+      </c>
+      <c r="F38" t="n">
+        <v>32</v>
+      </c>
+      <c r="G38" t="n">
+        <v>20</v>
+      </c>
+      <c r="H38" t="b">
+        <v>1</v>
+      </c>
+      <c r="I38" t="n">
+        <v>6</v>
+      </c>
+      <c r="J38" t="n">
+        <v>4</v>
+      </c>
+      <c r="K38" t="n">
+        <v>3</v>
+      </c>
+      <c r="L38" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="M38" t="inlineStr">
+        <is>
+          <t>Tanh</t>
+        </is>
+      </c>
+      <c r="N38" t="b">
+        <v>0</v>
+      </c>
+      <c r="O38" t="n">
+        <v>0</v>
+      </c>
+      <c r="P38" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q38" t="inlineStr"/>
+      <c r="R38" t="n">
+        <v>20</v>
+      </c>
+      <c r="S38" t="n">
+        <v>5</v>
+      </c>
+      <c r="T38" t="n">
+        <v>0.0001192906783933026</v>
+      </c>
+      <c r="U38" t="n">
+        <v>0.00105296271098307</v>
+      </c>
+      <c r="V38" t="n">
+        <v>3.640390157699585</v>
+      </c>
+      <c r="W38" t="n">
+        <v>4.423426628112793</v>
+      </c>
+      <c r="X38" t="n">
+        <v>2.494117021560669</v>
+      </c>
+      <c r="Y38" t="inlineStr">
+        <is>
+          <t>test run with classical only layer</t>
+        </is>
+      </c>
+      <c r="Z38" t="inlineStr">
         <is>
           <t>AAPL, MSFT, GOOGL</t>
         </is>

</xml_diff>

<commit_message>
upd best model more epochs
</commit_message>
<xml_diff>
--- a/model/qml_experiment_log.xlsx
+++ b/model/qml_experiment_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Z38"/>
+  <dimension ref="A1:Z39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3621,6 +3621,94 @@
         </is>
       </c>
     </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Auto-log: Q=6, D=4, Skip=add</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>0</v>
+      </c>
+      <c r="D39" t="n">
+        <v>4</v>
+      </c>
+      <c r="E39" t="n">
+        <v>0</v>
+      </c>
+      <c r="F39" t="n">
+        <v>32</v>
+      </c>
+      <c r="G39" t="n">
+        <v>20</v>
+      </c>
+      <c r="H39" t="b">
+        <v>1</v>
+      </c>
+      <c r="I39" t="n">
+        <v>6</v>
+      </c>
+      <c r="J39" t="n">
+        <v>4</v>
+      </c>
+      <c r="K39" t="n">
+        <v>3</v>
+      </c>
+      <c r="L39" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="M39" t="inlineStr">
+        <is>
+          <t>Tanh</t>
+        </is>
+      </c>
+      <c r="N39" t="b">
+        <v>0</v>
+      </c>
+      <c r="O39" t="n">
+        <v>0</v>
+      </c>
+      <c r="P39" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q39" t="inlineStr"/>
+      <c r="R39" t="n">
+        <v>40</v>
+      </c>
+      <c r="S39" t="n">
+        <v>10</v>
+      </c>
+      <c r="T39" t="n">
+        <v>8.380591476994363e-05</v>
+      </c>
+      <c r="U39" t="n">
+        <v>0.002030752476012493</v>
+      </c>
+      <c r="V39" t="n">
+        <v>2.565991401672363</v>
+      </c>
+      <c r="W39" t="n">
+        <v>3.171932220458984</v>
+      </c>
+      <c r="X39" t="n">
+        <v>1.774586319923401</v>
+      </c>
+      <c r="Y39" t="inlineStr">
+        <is>
+          <t>test run with classical only layer</t>
+        </is>
+      </c>
+      <c r="Z39" t="inlineStr">
+        <is>
+          <t>AAPL, MSFT, GOOGL</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>